<commit_message>
Added gesture module to automation
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_System_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_System_JS.xlsx
@@ -2653,10 +2653,9 @@
 ClickRunTest(runtest_top_xpath);
 validate3;
 ClickRunTest(runtest_bottom_xpath);
-wait(5);
 UIAutomatorScreenshot(VT300_076);
-validate4;
-press_Key(Back);</t>
+press_Key(Back);
+validate4;</t>
   </si>
   <si>
     <t>validate1
@@ -2673,7 +2672,7 @@
 };
 validate4
 {
-UIAutomatorScreenshot=VT300_076
+validate_Screenshot=VT300_076
 };</t>
   </si>
 </sst>

</xml_diff>